<commit_message>
Added Logo, corrected for sizing. Updated theme to match logo colours
</commit_message>
<xml_diff>
--- a/website_content_creation/authors/Derek Chartrand/Author_form_DC.xlsx
+++ b/website_content_creation/authors/Derek Chartrand/Author_form_DC.xlsx
@@ -101,9 +101,6 @@
     <t>Derek Chartrand</t>
   </si>
   <si>
-    <t>Chemisty Lab Technician</t>
-  </si>
-  <si>
     <t>derek.chartrand@canada.ca</t>
   </si>
   <si>
@@ -114,6 +111,9 @@
   </si>
   <si>
     <t>Watershed Ecology Team</t>
+  </si>
+  <si>
+    <t>Chemistry Lab Technician</t>
   </si>
 </sst>
 </file>
@@ -386,6 +386,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -395,7 +396,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -680,7 +680,7 @@
   <dimension ref="A1:C36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -713,7 +713,7 @@
         <v>14</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
@@ -727,7 +727,7 @@
         <v>2</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
@@ -752,15 +752,15 @@
         <v>18</v>
       </c>
       <c r="B10" s="14" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" s="15" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" s="18" t="s">
+      <c r="B11" t="s">
         <v>28</v>
-      </c>
-      <c r="B11" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -769,11 +769,11 @@
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13" s="15" t="s">
+      <c r="A13" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="B13" s="16"/>
-      <c r="C13" s="17"/>
+      <c r="B13" s="17"/>
+      <c r="C13" s="18"/>
     </row>
     <row r="14" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="5" t="s">
@@ -813,10 +813,10 @@
     </row>
     <row r="20" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A21" s="15" t="s">
+      <c r="A21" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="B21" s="17"/>
+      <c r="B21" s="18"/>
     </row>
     <row r="22" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="5" t="s">

</xml_diff>